<commit_message>
update flow add sub bag
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/Report.xlsx
+++ b/src/main/resources/input_excel_file/booking/Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="1" activeTab="4"/>
+    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="1" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Revenue_Detail_Report" sheetId="10" r:id="rId1"/>
@@ -499,7 +499,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="332" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="342" uniqueCount="108">
   <si>
     <t>tc_id</t>
   </si>
@@ -781,6 +781,12 @@
   </si>
   <si>
     <t>Kiểm tra danh sách doanh thu booking khách lẻ player 1</t>
+  </si>
+  <si>
+    <t>REPORT_VST_PLAYER1_001</t>
+  </si>
+  <si>
+    <t>Kiểm tra danh sách doanh thu booking khách lẻ player 1 khi add main - sub</t>
   </si>
   <si>
     <t>REPORT_AGENCY_PLAYER2</t>
@@ -1003,12 +1009,12 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -2421,10 +2427,610 @@
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
+  <dimension ref="A1:AV4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="V15" sqref="V15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="3"/>
+  <cols>
+    <col min="1" max="1" width="27.2190476190476" style="1" customWidth="1"/>
+    <col min="2" max="2" width="31.9333333333333" style="1" customWidth="1"/>
+    <col min="3" max="3" width="19.4857142857143" style="1" customWidth="1"/>
+    <col min="4" max="4" width="30" style="1" customWidth="1"/>
+    <col min="5" max="5" width="21" style="1" customWidth="1"/>
+    <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
+    <col min="7" max="7" width="24.7047619047619" style="1" customWidth="1"/>
+    <col min="8" max="8" width="16.7142857142857" style="1" customWidth="1"/>
+    <col min="9" max="9" width="23.1904761904762" style="1" customWidth="1"/>
+    <col min="10" max="10" width="21.5714285714286" style="1" customWidth="1"/>
+    <col min="11" max="11" width="21.4285714285714" style="1" customWidth="1"/>
+    <col min="12" max="12" width="17.8380952380952" style="1" customWidth="1"/>
+    <col min="13" max="13" width="17.8380952380952" style="2" customWidth="1"/>
+    <col min="14" max="15" width="17.8380952380952" style="1" customWidth="1"/>
+    <col min="16" max="16" width="17.8380952380952" style="2" customWidth="1"/>
+    <col min="17" max="17" width="36.1333333333333" style="1" customWidth="1"/>
+    <col min="18" max="18" width="15.2857142857143" style="1" customWidth="1"/>
+    <col min="19" max="19" width="13.447619047619" style="1" customWidth="1"/>
+    <col min="20" max="21" width="21.1619047619048" style="1" customWidth="1"/>
+    <col min="22" max="22" width="22.847619047619" style="1" customWidth="1"/>
+    <col min="23" max="25" width="18.8095238095238" style="1" customWidth="1"/>
+    <col min="26" max="36" width="26.7142857142857" style="1" customWidth="1"/>
+    <col min="37" max="46" width="22.0190476190476" style="1" customWidth="1"/>
+    <col min="47" max="47" width="29.4095238095238" style="1" customWidth="1"/>
+    <col min="48" max="48" width="22.0190476190476" style="1" customWidth="1"/>
+    <col min="49" max="16384" width="9.14285714285714" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:48">
+      <c r="A1" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="O1" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="P1" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="Q1" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="R1" s="11" t="s">
+        <v>17</v>
+      </c>
+      <c r="S1" s="12" t="s">
+        <v>59</v>
+      </c>
+      <c r="T1" s="12" t="s">
+        <v>60</v>
+      </c>
+      <c r="U1" s="12" t="s">
+        <v>61</v>
+      </c>
+      <c r="V1" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="W1" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="X1" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="Y1" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z1" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="AA1" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="AB1" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="AC1" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="AD1" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="AE1" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="AF1" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="AG1" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="AH1" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="AI1" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="AJ1" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="AK1" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="AL1" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="AM1" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="AN1" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="AO1" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="AP1" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="AQ1" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="AR1" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="AS1" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="AT1" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="AU1" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="AV1" s="11" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:48">
+      <c r="A2" s="5" t="s">
+        <v>89</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>90</v>
+      </c>
+      <c r="C2" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D2" s="6"/>
+      <c r="E2" s="8">
+        <v>20</v>
+      </c>
+      <c r="F2" s="8">
+        <v>1</v>
+      </c>
+      <c r="G2" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H2" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I2" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J2" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L2" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M2" s="8"/>
+      <c r="N2" s="8"/>
+      <c r="O2" s="8"/>
+      <c r="P2" s="8"/>
+      <c r="Q2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="R2" s="8">
+        <v>200</v>
+      </c>
+      <c r="S2" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="T2" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="U2" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="V2" s="13">
+        <v>0</v>
+      </c>
+      <c r="W2" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="X2" s="8">
+        <v>400000</v>
+      </c>
+      <c r="Y2" s="8">
+        <v>600000</v>
+      </c>
+      <c r="Z2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AL2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AR2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU2" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV2" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:48">
+      <c r="A3" s="5" t="s">
+        <v>92</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>93</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D3" s="6"/>
+      <c r="E3" s="8">
+        <v>20</v>
+      </c>
+      <c r="F3" s="8">
+        <v>1</v>
+      </c>
+      <c r="G3" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H3" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L3" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M3" s="8"/>
+      <c r="N3" s="8"/>
+      <c r="O3" s="8"/>
+      <c r="P3" s="8"/>
+      <c r="Q3" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="R3" s="8">
+        <v>200</v>
+      </c>
+      <c r="S3" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="T3" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="U3" s="13">
+        <v>0</v>
+      </c>
+      <c r="V3" s="13">
+        <v>8000000</v>
+      </c>
+      <c r="W3" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="X3" s="8">
+        <v>400000</v>
+      </c>
+      <c r="Y3" s="8">
+        <v>600000</v>
+      </c>
+      <c r="Z3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK3" s="8">
+        <v>1600000</v>
+      </c>
+      <c r="AL3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AR3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU3" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV3" s="8">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" s="1" customFormat="1" ht="61" customHeight="1" spans="1:48">
+      <c r="A4" s="5" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>95</v>
+      </c>
+      <c r="C4" s="7" t="s">
+        <v>52</v>
+      </c>
+      <c r="D4" s="6"/>
+      <c r="E4" s="8">
+        <v>20</v>
+      </c>
+      <c r="F4" s="8">
+        <v>1</v>
+      </c>
+      <c r="G4" s="8" t="s">
+        <v>53</v>
+      </c>
+      <c r="H4" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="I4" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="J4" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="K4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="L4" s="9" t="s">
+        <v>57</v>
+      </c>
+      <c r="M4" s="8"/>
+      <c r="N4" s="8"/>
+      <c r="O4" s="8"/>
+      <c r="P4" s="8"/>
+      <c r="Q4" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="R4" s="8">
+        <v>200</v>
+      </c>
+      <c r="S4" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="T4" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="U4" s="13">
+        <v>0</v>
+      </c>
+      <c r="V4" s="13">
+        <v>2000000</v>
+      </c>
+      <c r="W4" s="13">
+        <v>1000000</v>
+      </c>
+      <c r="X4" s="8">
+        <v>400000</v>
+      </c>
+      <c r="Y4" s="8">
+        <v>600000</v>
+      </c>
+      <c r="Z4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AA4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AB4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AC4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AD4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AE4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AF4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AG4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AH4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AI4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AJ4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AK4" s="8">
+        <v>1600000</v>
+      </c>
+      <c r="AL4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AM4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AN4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AO4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AP4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AQ4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AR4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AS4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AT4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AU4" s="8">
+        <v>0</v>
+      </c>
+      <c r="AV4" s="8">
+        <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+  <legacyDrawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
   <dimension ref="A1:AV3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="Y14" sqref="Y14"/>
+      <selection activeCell="A3" sqref="$A3:$XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="2"/>
@@ -2605,10 +3211,10 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:48">
       <c r="A2" s="5" t="s">
-        <v>89</v>
+        <v>96</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>90</v>
+        <v>97</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>52</v>
@@ -2741,474 +3347,10 @@
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:48">
       <c r="A3" s="5" t="s">
-        <v>92</v>
+        <v>98</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>93</v>
-      </c>
-      <c r="C3" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="8">
-        <v>20</v>
-      </c>
-      <c r="F3" s="8">
-        <v>1</v>
-      </c>
-      <c r="G3" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H3" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I3" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J3" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="L3" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="M3" s="8"/>
-      <c r="N3" s="8"/>
-      <c r="O3" s="8"/>
-      <c r="P3" s="8"/>
-      <c r="Q3" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="R3" s="8">
-        <v>200</v>
-      </c>
-      <c r="S3" s="13">
-        <v>2000000</v>
-      </c>
-      <c r="T3" s="13">
-        <v>2000000</v>
-      </c>
-      <c r="U3" s="13">
-        <v>0</v>
-      </c>
-      <c r="V3" s="13">
-        <v>8000000</v>
-      </c>
-      <c r="W3" s="13">
-        <v>1000000</v>
-      </c>
-      <c r="X3" s="8">
-        <v>400000</v>
-      </c>
-      <c r="Y3" s="8">
-        <v>600000</v>
-      </c>
-      <c r="Z3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK3" s="8">
-        <v>1600000</v>
-      </c>
-      <c r="AL3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU3" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV3" s="8">
-        <v>0</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
-  <headerFooter/>
-  <legacyDrawing r:id="rId2"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
-  <sheetPr/>
-  <dimension ref="A1:AV3"/>
-  <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="V4" sqref="V4"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="2"/>
-  <cols>
-    <col min="1" max="1" width="27.2190476190476" style="1" customWidth="1"/>
-    <col min="2" max="2" width="31.9333333333333" style="1" customWidth="1"/>
-    <col min="3" max="3" width="19.4857142857143" style="1" customWidth="1"/>
-    <col min="4" max="4" width="30" style="1" customWidth="1"/>
-    <col min="5" max="5" width="21" style="1" customWidth="1"/>
-    <col min="6" max="6" width="22.4285714285714" style="1" customWidth="1"/>
-    <col min="7" max="7" width="24.7047619047619" style="1" customWidth="1"/>
-    <col min="8" max="8" width="16.7142857142857" style="1" customWidth="1"/>
-    <col min="9" max="9" width="23.1904761904762" style="1" customWidth="1"/>
-    <col min="10" max="10" width="21.5714285714286" style="1" customWidth="1"/>
-    <col min="11" max="11" width="21.4285714285714" style="1" customWidth="1"/>
-    <col min="12" max="12" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="13" max="13" width="17.8380952380952" style="2" customWidth="1"/>
-    <col min="14" max="15" width="17.8380952380952" style="1" customWidth="1"/>
-    <col min="16" max="16" width="17.8380952380952" style="2" customWidth="1"/>
-    <col min="17" max="17" width="36.1333333333333" style="1" customWidth="1"/>
-    <col min="18" max="18" width="15.2857142857143" style="1" customWidth="1"/>
-    <col min="19" max="19" width="13.447619047619" style="1" customWidth="1"/>
-    <col min="20" max="21" width="21.1619047619048" style="1" customWidth="1"/>
-    <col min="22" max="22" width="22.847619047619" style="1" customWidth="1"/>
-    <col min="23" max="25" width="18.8095238095238" style="1" customWidth="1"/>
-    <col min="26" max="36" width="26.7142857142857" style="1" customWidth="1"/>
-    <col min="37" max="46" width="22.0190476190476" style="1" customWidth="1"/>
-    <col min="47" max="47" width="29.4095238095238" style="1" customWidth="1"/>
-    <col min="48" max="48" width="22.0190476190476" style="1" customWidth="1"/>
-    <col min="49" max="16384" width="9.14285714285714" style="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" s="1" customFormat="1" ht="47" customHeight="1" spans="1:48">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="D1" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="E1" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="F1" s="4" t="s">
-        <v>5</v>
-      </c>
-      <c r="G1" s="4" t="s">
-        <v>6</v>
-      </c>
-      <c r="H1" s="4" t="s">
-        <v>7</v>
-      </c>
-      <c r="I1" s="4" t="s">
-        <v>8</v>
-      </c>
-      <c r="J1" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="K1" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="L1" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="M1" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="N1" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="O1" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="P1" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="Q1" s="10" t="s">
-        <v>16</v>
-      </c>
-      <c r="R1" s="11" t="s">
-        <v>17</v>
-      </c>
-      <c r="S1" s="12" t="s">
-        <v>59</v>
-      </c>
-      <c r="T1" s="12" t="s">
-        <v>60</v>
-      </c>
-      <c r="U1" s="12" t="s">
-        <v>61</v>
-      </c>
-      <c r="V1" s="12" t="s">
-        <v>62</v>
-      </c>
-      <c r="W1" s="11" t="s">
-        <v>63</v>
-      </c>
-      <c r="X1" s="11" t="s">
-        <v>64</v>
-      </c>
-      <c r="Y1" s="11" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z1" s="14" t="s">
-        <v>66</v>
-      </c>
-      <c r="AA1" s="14" t="s">
-        <v>67</v>
-      </c>
-      <c r="AB1" s="14" t="s">
-        <v>68</v>
-      </c>
-      <c r="AC1" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="AD1" s="14" t="s">
-        <v>70</v>
-      </c>
-      <c r="AE1" s="14" t="s">
-        <v>71</v>
-      </c>
-      <c r="AF1" s="14" t="s">
-        <v>72</v>
-      </c>
-      <c r="AG1" s="14" t="s">
-        <v>73</v>
-      </c>
-      <c r="AH1" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="AI1" s="14" t="s">
-        <v>75</v>
-      </c>
-      <c r="AJ1" s="14" t="s">
-        <v>76</v>
-      </c>
-      <c r="AK1" s="11" t="s">
-        <v>77</v>
-      </c>
-      <c r="AL1" s="11" t="s">
-        <v>78</v>
-      </c>
-      <c r="AM1" s="11" t="s">
-        <v>79</v>
-      </c>
-      <c r="AN1" s="11" t="s">
-        <v>80</v>
-      </c>
-      <c r="AO1" s="11" t="s">
-        <v>81</v>
-      </c>
-      <c r="AP1" s="11" t="s">
-        <v>82</v>
-      </c>
-      <c r="AQ1" s="11" t="s">
-        <v>83</v>
-      </c>
-      <c r="AR1" s="11" t="s">
-        <v>84</v>
-      </c>
-      <c r="AS1" s="11" t="s">
-        <v>85</v>
-      </c>
-      <c r="AT1" s="11" t="s">
-        <v>86</v>
-      </c>
-      <c r="AU1" s="11" t="s">
-        <v>87</v>
-      </c>
-      <c r="AV1" s="11" t="s">
-        <v>88</v>
-      </c>
-    </row>
-    <row r="2" s="1" customFormat="1" customHeight="1" spans="1:48">
-      <c r="A2" s="5" t="s">
-        <v>94</v>
-      </c>
-      <c r="B2" s="6" t="s">
-        <v>95</v>
-      </c>
-      <c r="C2" s="7" t="s">
-        <v>52</v>
-      </c>
-      <c r="D2" s="6"/>
-      <c r="E2" s="8">
-        <v>20</v>
-      </c>
-      <c r="F2" s="8">
-        <v>1</v>
-      </c>
-      <c r="G2" s="8" t="s">
-        <v>53</v>
-      </c>
-      <c r="H2" s="8" t="s">
-        <v>54</v>
-      </c>
-      <c r="I2" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="J2" s="5" t="s">
-        <v>56</v>
-      </c>
-      <c r="K2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" s="9" t="s">
-        <v>57</v>
-      </c>
-      <c r="M2" s="8"/>
-      <c r="N2" s="8"/>
-      <c r="O2" s="8"/>
-      <c r="P2" s="8"/>
-      <c r="Q2" s="6" t="s">
-        <v>91</v>
-      </c>
-      <c r="R2" s="8">
-        <v>200</v>
-      </c>
-      <c r="S2" s="13">
-        <v>2000000</v>
-      </c>
-      <c r="T2" s="13">
-        <v>2000000</v>
-      </c>
-      <c r="U2" s="13">
-        <v>2000000</v>
-      </c>
-      <c r="V2" s="13">
-        <v>0</v>
-      </c>
-      <c r="W2" s="13">
-        <v>1000000</v>
-      </c>
-      <c r="X2" s="8">
-        <v>400000</v>
-      </c>
-      <c r="Y2" s="8">
-        <v>600000</v>
-      </c>
-      <c r="Z2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AA2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AB2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AC2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AD2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AE2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AF2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AG2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AH2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AI2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AJ2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AK2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AL2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AM2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AN2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AO2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AP2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AQ2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AR2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AS2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AT2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AU2" s="8">
-        <v>0</v>
-      </c>
-      <c r="AV2" s="8">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" s="1" customFormat="1" customHeight="1" spans="1:48">
-      <c r="A3" s="5" t="s">
-        <v>96</v>
-      </c>
-      <c r="B3" s="6" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>52</v>
@@ -3533,10 +3675,10 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:48">
       <c r="A2" s="5" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>52</v>
@@ -3669,10 +3811,10 @@
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:48">
       <c r="A3" s="5" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>52</v>
@@ -3815,8 +3957,8 @@
   <sheetPr/>
   <dimension ref="A1:AV3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="G1" workbookViewId="0">
-      <selection activeCell="P17" sqref="P17"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="F13" sqref="F13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="2"/>
@@ -3997,10 +4139,10 @@
     </row>
     <row r="2" s="1" customFormat="1" customHeight="1" spans="1:48">
       <c r="A2" s="5" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
       <c r="B2" s="6" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="C2" s="7" t="s">
         <v>52</v>
@@ -4133,10 +4275,10 @@
     </row>
     <row r="3" s="1" customFormat="1" customHeight="1" spans="1:48">
       <c r="A3" s="5" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="C3" s="7" t="s">
         <v>52</v>

</xml_diff>

<commit_message>
update api get for make template gen test script
</commit_message>
<xml_diff>
--- a/src/main/resources/input_excel_file/booking/Report.xlsx
+++ b/src/main/resources/input_excel_file/booking/Report.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="28800" windowHeight="12180" firstSheet="1" activeTab="1"/>
+    <workbookView windowWidth="28800" windowHeight="12180" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Revenue_Detail_Report" sheetId="10" r:id="rId1"/>
@@ -513,40 +513,40 @@
     <t>input_placeholders</t>
   </si>
   <si>
-    <t>limit</t>
-  </si>
-  <si>
-    <t>page</t>
-  </si>
-  <si>
-    <t>sort_by</t>
-  </si>
-  <si>
-    <t>sort_dir</t>
-  </si>
-  <si>
-    <t>partner_uid</t>
-  </si>
-  <si>
-    <t>course_uid</t>
-  </si>
-  <si>
-    <t>date_from</t>
-  </si>
-  <si>
-    <t>date_to</t>
-  </si>
-  <si>
-    <t>guest_style</t>
-  </si>
-  <si>
-    <t>bag</t>
-  </si>
-  <si>
-    <t>transaction_code</t>
-  </si>
-  <si>
-    <t>revenue_type</t>
+    <t>q_limit</t>
+  </si>
+  <si>
+    <t>q_page</t>
+  </si>
+  <si>
+    <t>q_sort_by</t>
+  </si>
+  <si>
+    <t>q_sort_dir</t>
+  </si>
+  <si>
+    <t>q_partner_uid</t>
+  </si>
+  <si>
+    <t>q_course_uid</t>
+  </si>
+  <si>
+    <t>q_date_from</t>
+  </si>
+  <si>
+    <t>q_date_to</t>
+  </si>
+  <si>
+    <t>q_guest_style</t>
+  </si>
+  <si>
+    <t>q_bag</t>
+  </si>
+  <si>
+    <t>q_transaction_code</t>
+  </si>
+  <si>
+    <t>q_revenue_type</t>
   </si>
   <si>
     <t>expected_validation_data</t>
@@ -1009,12 +1009,12 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
     </font>
     <font>
-      <b/>
       <sz val="9"/>
       <name val="Times New Roman"/>
       <charset val="0"/>
@@ -2090,8 +2090,8 @@
   <sheetPr/>
   <dimension ref="A1:AX2"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="1"/>
@@ -2429,8 +2429,8 @@
   <sheetPr/>
   <dimension ref="A1:AV4"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="V15" sqref="V15"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="E1" sqref="E1:P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="3"/>
@@ -3030,7 +3030,7 @@
   <dimension ref="A1:AV3"/>
   <sheetViews>
     <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A3" sqref="$A3:$XFD3"/>
+      <selection activeCell="F16" sqref="F16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="2"/>
@@ -3493,8 +3493,8 @@
   <sheetPr/>
   <dimension ref="A1:AV3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="V11" sqref="V11"/>
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="2"/>
@@ -3957,8 +3957,8 @@
   <sheetPr/>
   <dimension ref="A1:AV3"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="F13" sqref="F13"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.14285714285714" defaultRowHeight="30" customHeight="1" outlineLevelRow="2"/>

</xml_diff>